<commit_message>
So many more plots and model and plots and model and a draft or two
</commit_message>
<xml_diff>
--- a/Data/mich_tree_additions.xlsx
+++ b/Data/mich_tree_additions.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2880" windowWidth="28040" windowHeight="16720"/>
+    <workbookView xWindow="30000" yWindow="1180" windowWidth="28040" windowHeight="16720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="608" uniqueCount="205">
   <si>
     <t>name</t>
   </si>
@@ -622,6 +622,24 @@
   </si>
   <si>
     <t>Bignoniaceae</t>
+  </si>
+  <si>
+    <t>moist_use</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -980,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G148"/>
+  <dimension ref="A1:I148"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="D120" sqref="D120"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="108" workbookViewId="0">
+      <selection activeCell="E153" sqref="E153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -992,7 +1010,7 @@
     <col min="5" max="5" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>161</v>
       </c>
@@ -1014,8 +1032,11 @@
       <c r="G1" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>162</v>
       </c>
@@ -1028,8 +1049,11 @@
       <c r="G2">
         <v>23.69</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>163</v>
       </c>
@@ -1045,8 +1069,11 @@
       <c r="G3">
         <v>103</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>163</v>
       </c>
@@ -1065,8 +1092,11 @@
       <c r="G4">
         <v>79</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>164</v>
       </c>
@@ -1085,8 +1115,11 @@
       <c r="G5">
         <v>57.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H5" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>165</v>
       </c>
@@ -1108,8 +1141,11 @@
       <c r="G6">
         <v>847</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H6" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>166</v>
       </c>
@@ -1128,8 +1164,11 @@
       <c r="G7">
         <v>2.85</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H7" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>167</v>
       </c>
@@ -1145,8 +1184,11 @@
       <c r="G8">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>168</v>
       </c>
@@ -1165,8 +1207,11 @@
       <c r="G9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -1185,8 +1230,11 @@
       <c r="G10">
         <v>108.32</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -1202,8 +1250,14 @@
       <c r="G11">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H11" t="s">
+        <v>200</v>
+      </c>
+      <c r="I11" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -1216,8 +1270,11 @@
       <c r="E12">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -1233,8 +1290,14 @@
       <c r="G13">
         <v>1.2</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -1250,8 +1313,11 @@
       <c r="G14">
         <v>23.5</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>170</v>
       </c>
@@ -1267,8 +1333,11 @@
       <c r="G15">
         <v>25.2</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>170</v>
       </c>
@@ -1284,8 +1353,11 @@
       <c r="G16">
         <v>36.225000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>170</v>
       </c>
@@ -1301,8 +1373,11 @@
       <c r="G17">
         <v>79</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H17" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>171</v>
       </c>
@@ -1321,8 +1396,11 @@
       <c r="G18">
         <v>108.1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>171</v>
       </c>
@@ -1341,8 +1419,11 @@
       <c r="G19">
         <v>34</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H19" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -1361,8 +1442,11 @@
       <c r="G20">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H20" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>173</v>
       </c>
@@ -1381,8 +1465,11 @@
       <c r="G21">
         <v>6701</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>173</v>
       </c>
@@ -1401,8 +1488,11 @@
       <c r="G22">
         <v>23.2</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H22" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>173</v>
       </c>
@@ -1421,8 +1511,11 @@
       <c r="G23">
         <v>125.5</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>173</v>
       </c>
@@ -1441,8 +1534,11 @@
       <c r="G24">
         <v>37.299999999999997</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>173</v>
       </c>
@@ -1461,8 +1557,11 @@
       <c r="G25">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>173</v>
       </c>
@@ -1481,8 +1580,11 @@
       <c r="G26">
         <v>201.5</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H26" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>173</v>
       </c>
@@ -1501,8 +1603,11 @@
       <c r="G27" s="1">
         <v>23.7</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H27" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>173</v>
       </c>
@@ -1521,8 +1626,11 @@
       <c r="G28">
         <v>55.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>174</v>
       </c>
@@ -1544,8 +1652,11 @@
       <c r="G29">
         <v>29.4</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H29" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>175</v>
       </c>
@@ -1561,8 +1672,11 @@
       <c r="G30">
         <v>21.5</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>176</v>
       </c>
@@ -1575,8 +1689,11 @@
       <c r="G31">
         <v>16.5</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H31" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>177</v>
       </c>
@@ -1592,8 +1709,11 @@
       <c r="G32">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H32" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>178</v>
       </c>
@@ -1609,8 +1729,11 @@
       <c r="G33">
         <v>3.01</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>178</v>
       </c>
@@ -1626,8 +1749,11 @@
       <c r="G34">
         <v>1.67</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H34" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>178</v>
       </c>
@@ -1646,8 +1772,11 @@
       <c r="G35">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H35" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>178</v>
       </c>
@@ -1663,8 +1792,11 @@
       <c r="G36">
         <v>1.1200000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H36" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>178</v>
       </c>
@@ -1683,8 +1815,11 @@
       <c r="G37">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H37" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>178</v>
       </c>
@@ -1703,8 +1838,11 @@
       <c r="G38">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H38" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>178</v>
       </c>
@@ -1720,8 +1858,11 @@
       <c r="G39">
         <v>0.161</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>178</v>
       </c>
@@ -1734,8 +1875,11 @@
       <c r="E40">
         <v>4</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>178</v>
       </c>
@@ -1754,8 +1898,11 @@
       <c r="G41">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H41" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>178</v>
       </c>
@@ -1774,8 +1921,11 @@
       <c r="G42">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H42" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>178</v>
       </c>
@@ -1791,8 +1941,11 @@
       <c r="G43">
         <v>0.17299999999999999</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H43" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>178</v>
       </c>
@@ -1808,8 +1961,11 @@
       <c r="G44">
         <v>0.24199999999999999</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>178</v>
       </c>
@@ -1828,8 +1984,11 @@
       <c r="G45">
         <v>0.16</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>178</v>
       </c>
@@ -1845,8 +2004,14 @@
       <c r="G46">
         <v>4.1000000000000002E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H46" t="s">
+        <v>202</v>
+      </c>
+      <c r="I46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>178</v>
       </c>
@@ -1859,8 +2024,11 @@
       <c r="E47">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H47" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>178</v>
       </c>
@@ -1876,8 +2044,11 @@
       <c r="G48">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H48" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>179</v>
       </c>
@@ -1896,8 +2067,11 @@
       <c r="G49">
         <v>266</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H49" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>179</v>
       </c>
@@ -1916,8 +2090,11 @@
       <c r="G50">
         <v>3467.3</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H50" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>179</v>
       </c>
@@ -1936,8 +2113,11 @@
       <c r="G51">
         <v>1742</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H51" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>179</v>
       </c>
@@ -1956,8 +2136,11 @@
       <c r="G52">
         <v>1192.17</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H52" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>179</v>
       </c>
@@ -1976,8 +2159,11 @@
       <c r="G53">
         <v>1093.99</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H53" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>179</v>
       </c>
@@ -1996,8 +2182,11 @@
       <c r="G54">
         <v>4540.46</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H54" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>179</v>
       </c>
@@ -2016,8 +2205,11 @@
       <c r="G55">
         <v>1087</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H55" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>179</v>
       </c>
@@ -2036,8 +2228,11 @@
       <c r="G56">
         <v>1852</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H56" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>179</v>
       </c>
@@ -2056,8 +2251,11 @@
       <c r="G57">
         <v>3143</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H57" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>179</v>
       </c>
@@ -2076,8 +2274,11 @@
       <c r="G58">
         <v>3459</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H58" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>179</v>
       </c>
@@ -2096,8 +2297,11 @@
       <c r="G59">
         <v>6145</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H59" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>179</v>
       </c>
@@ -2116,8 +2320,11 @@
       <c r="G60">
         <v>2997</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H60" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>180</v>
       </c>
@@ -2127,8 +2334,11 @@
       <c r="D61" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H61" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>180</v>
       </c>
@@ -2144,8 +2354,11 @@
       <c r="G62">
         <v>1.57</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H62" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>181</v>
       </c>
@@ -2164,8 +2377,11 @@
       <c r="G63">
         <v>15141</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H63" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>181</v>
       </c>
@@ -2181,8 +2397,11 @@
       <c r="G64">
         <v>4401</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H64" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>181</v>
       </c>
@@ -2201,8 +2420,11 @@
       <c r="G65">
         <v>2797.6</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H65" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>181</v>
       </c>
@@ -2221,8 +2443,11 @@
       <c r="G66">
         <v>3502</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H66" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>181</v>
       </c>
@@ -2241,8 +2466,11 @@
       <c r="G67">
         <v>14026</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H67" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>181</v>
       </c>
@@ -2261,8 +2489,11 @@
       <c r="G68">
         <v>11303</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>182</v>
       </c>
@@ -2278,8 +2509,11 @@
       <c r="G69">
         <v>0.50880000000000003</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>182</v>
       </c>
@@ -2298,8 +2532,11 @@
       <c r="G70">
         <v>0.51759999999999995</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H70" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>182</v>
       </c>
@@ -2318,8 +2555,11 @@
       <c r="G71">
         <v>1.0429999999999999</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H71" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>182</v>
       </c>
@@ -2335,8 +2575,11 @@
       <c r="G72">
         <v>785.1</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H72" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>182</v>
       </c>
@@ -2352,8 +2595,11 @@
       <c r="G73">
         <v>833.3</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H73" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>182</v>
       </c>
@@ -2372,8 +2618,11 @@
       <c r="G74">
         <v>15.41</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H74" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>182</v>
       </c>
@@ -2392,8 +2641,11 @@
       <c r="G75">
         <v>26</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H75" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>182</v>
       </c>
@@ -2412,8 +2664,11 @@
       <c r="G76">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H76" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>182</v>
       </c>
@@ -2432,8 +2687,11 @@
       <c r="G77">
         <v>1.24</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H77" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>182</v>
       </c>
@@ -2449,8 +2707,11 @@
       <c r="G78">
         <v>0.59719999999999995</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H78" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>182</v>
       </c>
@@ -2469,8 +2730,11 @@
       <c r="G79">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H79" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>182</v>
       </c>
@@ -2489,8 +2753,11 @@
       <c r="G80">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H80" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>183</v>
       </c>
@@ -2506,8 +2773,11 @@
       <c r="G81">
         <v>20.6</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H81" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>183</v>
       </c>
@@ -2523,8 +2793,11 @@
       <c r="G82">
         <v>10.83</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H82" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>183</v>
       </c>
@@ -2540,8 +2813,11 @@
       <c r="G83">
         <v>3.49</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H83" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>184</v>
       </c>
@@ -2557,8 +2833,11 @@
       <c r="G84">
         <v>19.3</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H84" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>184</v>
       </c>
@@ -2574,8 +2853,11 @@
       <c r="G85">
         <v>8.8958999999999993</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>185</v>
       </c>
@@ -2594,8 +2876,11 @@
       <c r="G86">
         <v>60.5</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H86" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>185</v>
       </c>
@@ -2614,8 +2899,11 @@
       <c r="G87">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H87" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>185</v>
       </c>
@@ -2634,8 +2922,11 @@
       <c r="G88">
         <v>9.98</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H88" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>185</v>
       </c>
@@ -2654,8 +2945,11 @@
       <c r="G89">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H89" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>186</v>
       </c>
@@ -2674,8 +2968,11 @@
       <c r="G90">
         <v>126.4</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H90" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>187</v>
       </c>
@@ -2694,8 +2991,11 @@
       <c r="G91">
         <v>7</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H91" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>187</v>
       </c>
@@ -2714,8 +3014,11 @@
       <c r="G92">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H92" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>187</v>
       </c>
@@ -2734,8 +3037,11 @@
       <c r="G93">
         <v>32</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H93" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>188</v>
       </c>
@@ -2751,8 +3057,11 @@
       <c r="G94">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H94" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>188</v>
       </c>
@@ -2768,8 +3077,11 @@
       <c r="G95">
         <v>1.41</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H95" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>188</v>
       </c>
@@ -2785,8 +3097,14 @@
       <c r="G96">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H96" t="s">
+        <v>202</v>
+      </c>
+      <c r="I96" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>188</v>
       </c>
@@ -2802,8 +3120,11 @@
       <c r="G97">
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H97" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>188</v>
       </c>
@@ -2819,8 +3140,11 @@
       <c r="G98">
         <v>2.4700000000000002</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H98" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>188</v>
       </c>
@@ -2836,8 +3160,11 @@
       <c r="G99">
         <v>3.25</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H99" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>188</v>
       </c>
@@ -2856,8 +3183,11 @@
       <c r="G100">
         <v>10.93276</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H100" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>188</v>
       </c>
@@ -2870,8 +3200,11 @@
       <c r="G101">
         <v>2.9430000000000001</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H101" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>188</v>
       </c>
@@ -2884,8 +3217,11 @@
       <c r="G102">
         <v>17</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H102" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -2901,8 +3237,11 @@
       <c r="G103">
         <v>0.88119999999999998</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H103" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>188</v>
       </c>
@@ -2918,8 +3257,11 @@
       <c r="G104">
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H104" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>188</v>
       </c>
@@ -2935,8 +3277,14 @@
       <c r="E105">
         <v>4</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H105" t="s">
+        <v>200</v>
+      </c>
+      <c r="I105" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>188</v>
       </c>
@@ -2955,8 +3303,11 @@
       <c r="G106">
         <v>83.9</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H106" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>188</v>
       </c>
@@ -2975,8 +3326,11 @@
       <c r="G107">
         <v>81.099999999999994</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>188</v>
       </c>
@@ -2995,8 +3349,11 @@
       <c r="G108">
         <v>43.5</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H108" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>188</v>
       </c>
@@ -3012,8 +3369,11 @@
       <c r="G109">
         <v>155.33000000000001</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H109" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>188</v>
       </c>
@@ -3029,8 +3389,11 @@
       <c r="G110">
         <v>770</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H110" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>188</v>
       </c>
@@ -3046,8 +3409,11 @@
       <c r="G111">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H111" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>188</v>
       </c>
@@ -3066,8 +3432,11 @@
       <c r="G112">
         <v>5.65</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H112" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>188</v>
       </c>
@@ -3083,8 +3452,11 @@
       <c r="G113">
         <v>16.170000000000002</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H113" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>188</v>
       </c>
@@ -3094,8 +3466,11 @@
       <c r="G114">
         <v>163.80000000000001</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H114" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>188</v>
       </c>
@@ -3111,8 +3486,11 @@
       <c r="G115">
         <v>26.74</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H115" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>189</v>
       </c>
@@ -3128,8 +3506,11 @@
       <c r="G116">
         <v>24.6</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H116" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>189</v>
       </c>
@@ -3148,8 +3529,11 @@
       <c r="G117">
         <v>168.6</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H117" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>189</v>
       </c>
@@ -3168,8 +3552,11 @@
       <c r="G118">
         <v>19.2</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H118" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>190</v>
       </c>
@@ -3185,8 +3572,11 @@
       <c r="G119">
         <v>102</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H119" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>190</v>
       </c>
@@ -3208,8 +3598,11 @@
       <c r="G120">
         <v>50.6</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H120" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>190</v>
       </c>
@@ -3225,8 +3618,11 @@
       <c r="G121">
         <v>27.096299999999999</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H121" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>190</v>
       </c>
@@ -3242,8 +3638,11 @@
       <c r="G122">
         <v>35.43</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H122" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>190</v>
       </c>
@@ -3259,8 +3658,11 @@
       <c r="G123">
         <v>28.2</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H123" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>190</v>
       </c>
@@ -3276,8 +3678,11 @@
       <c r="G124">
         <v>46.381999999999998</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H124" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>191</v>
       </c>
@@ -3296,8 +3701,11 @@
       <c r="G125">
         <v>140</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H125" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>192</v>
       </c>
@@ -3313,8 +3721,11 @@
       <c r="G126">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H126" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>192</v>
       </c>
@@ -3330,8 +3741,11 @@
       <c r="G127">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H127" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>192</v>
       </c>
@@ -3347,8 +3761,11 @@
       <c r="G128">
         <v>1.63</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H128" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>192</v>
       </c>
@@ -3364,8 +3781,11 @@
       <c r="G129">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H129" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>193</v>
       </c>
@@ -3381,8 +3801,11 @@
       <c r="G130">
         <v>13.2</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H130" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>194</v>
       </c>
@@ -3398,8 +3821,11 @@
       <c r="G131">
         <v>2.7</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H131" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>194</v>
       </c>
@@ -3415,8 +3841,11 @@
       <c r="G132">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H132" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>194</v>
       </c>
@@ -3432,8 +3861,11 @@
       <c r="G133">
         <v>28.5</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H133" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>194</v>
       </c>
@@ -3449,8 +3881,14 @@
       <c r="G134">
         <v>39.299999999999997</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H134" t="s">
+        <v>200</v>
+      </c>
+      <c r="I134" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>194</v>
       </c>
@@ -3463,8 +3901,11 @@
       <c r="E135">
         <v>5</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H135" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>194</v>
       </c>
@@ -3480,8 +3921,11 @@
       <c r="G136">
         <v>75.95</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H136" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>195</v>
       </c>
@@ -3497,8 +3941,11 @@
       <c r="G137">
         <v>5.96</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H137" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>195</v>
       </c>
@@ -3514,8 +3961,11 @@
       <c r="G138">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H138" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>195</v>
       </c>
@@ -3531,8 +3981,11 @@
       <c r="G139">
         <v>3.06</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H139" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>196</v>
       </c>
@@ -3548,8 +4001,11 @@
       <c r="G140">
         <v>2.4</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H140" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>197</v>
       </c>
@@ -3568,8 +4024,11 @@
       <c r="G141">
         <v>142.32</v>
       </c>
-    </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H141" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>197</v>
       </c>
@@ -3588,8 +4047,11 @@
       <c r="G142">
         <v>32.299999999999997</v>
       </c>
-    </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H142" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>197</v>
       </c>
@@ -3608,8 +4070,11 @@
       <c r="G143">
         <v>37.299999999999997</v>
       </c>
-    </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H143" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>197</v>
       </c>
@@ -3628,8 +4093,11 @@
       <c r="G144">
         <v>55.3</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H144" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>197</v>
       </c>
@@ -3645,8 +4113,11 @@
       <c r="G145">
         <v>5.6</v>
       </c>
-    </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H145" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>197</v>
       </c>
@@ -3662,8 +4133,11 @@
       <c r="G146">
         <v>18.8</v>
       </c>
-    </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H146" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>198</v>
       </c>
@@ -3682,8 +4156,11 @@
       <c r="G147">
         <v>24.4</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H147" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>198</v>
       </c>
@@ -3701,6 +4178,9 @@
       </c>
       <c r="G148">
         <v>18.829999999999998</v>
+      </c>
+      <c r="H148" t="s">
+        <v>201</v>
       </c>
     </row>
   </sheetData>

</xml_diff>